<commit_message>
Added some bodies in Details.xslx
</commit_message>
<xml_diff>
--- a/HighResIcons/Details.xlsx
+++ b/HighResIcons/Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Andrea\Code\EDDiscovery\EDDiscoveryData\HighResIcons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C1AEE6-B989-4E19-A826-0BAD70A954CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1E153E-2FE5-42D9-BC86-09432470FA41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15360" yWindow="-1335" windowWidth="15360" windowHeight="9300" xr2:uid="{1C47AFF1-0F2E-4E80-9439-97C38743854E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C47AFF1-0F2E-4E80-9439-97C38743854E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="52">
   <si>
     <t>Class</t>
   </si>
@@ -174,15 +174,40 @@
   </si>
   <si>
     <t>oxigen</t>
+  </si>
+  <si>
+    <t>ELWv1</t>
+  </si>
+  <si>
+    <t>ELW</t>
+  </si>
+  <si>
+    <t>suitable for water based life</t>
+  </si>
+  <si>
+    <t>sulphur dioxide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -325,34 +350,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -671,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378DFCFD-A23B-459A-BDF7-1A47346AC4C8}">
   <dimension ref="B1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,11 +709,14 @@
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.140625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
@@ -701,576 +732,596 @@
       <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="4" t="s">
+      <c r="H2" s="4"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="10" t="s">
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="7" t="s">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="J3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="11">
         <v>285</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="11">
+        <v>148</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="11"/>
+    </row>
+    <row r="6" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="11">
+        <v>647</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="I6" s="11"/>
+      <c r="J6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="11"/>
+    </row>
+    <row r="7" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B7" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="11">
+        <v>321</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
+    <row r="8" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1">
-        <v>148</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="D8" s="11">
+        <v>221</v>
+      </c>
+      <c r="E8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="H8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="11"/>
+    </row>
+    <row r="9" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="1">
-        <v>647</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="D9" s="11">
+        <v>257</v>
+      </c>
+      <c r="E9" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H9" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="I9" s="11"/>
+      <c r="J9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1">
-        <v>321</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="D10" s="11">
+        <v>452</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="F10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B11" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="11">
+        <v>281</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L11" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="11">
+        <v>208</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L12" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="11">
+        <v>423</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="11">
+        <v>373</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L14" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B15" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="11">
+        <v>240</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="11"/>
+    </row>
+    <row r="16" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B16" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="11">
+        <v>259</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B17" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="11">
+        <v>257</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L17" s="11"/>
+    </row>
+    <row r="18" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="11">
+        <v>304</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L18" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="11">
+        <v>299</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L19" s="11"/>
+    </row>
+    <row r="20" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B20" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="11">
+        <v>297</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1">
-        <v>221</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1">
-        <v>257</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1">
-        <v>452</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" s="1">
-        <v>281</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="1">
-        <v>208</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1">
-        <v>423</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1">
-        <v>373</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="1">
-        <v>240</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L15" s="1"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="1">
-        <v>259</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="1">
-        <v>257</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="1">
-        <v>304</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="1">
-        <v>299</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
+      <c r="J20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="L20" s="11"/>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
@@ -1511,6 +1562,8 @@
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="J2:L2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add NWWv4, an ammonia water world
</commit_message>
<xml_diff>
--- a/HighResIcons/Details.xlsx
+++ b/HighResIcons/Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Andrea\Code\EDDiscovery\EDDiscoveryData\HighResIcons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA66C3C-FA2D-44BC-A783-41F132419571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A31D49B-7BDA-40A1-9DE8-CBB21E6C58D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C47AFF1-0F2E-4E80-9439-97C38743854E}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="57">
   <si>
     <t>Class</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Composition %</t>
+  </si>
+  <si>
+    <t>NWWv4</t>
   </si>
 </sst>
 </file>
@@ -709,10 +712,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378DFCFD-A23B-459A-BDF7-1A47346AC4C8}">
-  <dimension ref="B1:L39"/>
+  <dimension ref="B1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,48 +1272,46 @@
     </row>
     <row r="19" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D19" s="8">
-        <v>304</v>
+        <v>387</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J19" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K19" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L19" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="J19" s="8">
+        <v>67.3</v>
+      </c>
+      <c r="K19" s="8">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="L19" s="8"/>
     </row>
     <row r="20" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="8">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>14</v>
@@ -1322,42 +1323,44 @@
         <v>15</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="8"/>
+        <v>44</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="J20" s="8" t="s">
         <v>4</v>
       </c>
       <c r="K20" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L20" s="8"/>
+      <c r="L20" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D21" s="8">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="G21" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>22</v>
-      </c>
+      <c r="I21" s="8"/>
       <c r="J21" s="8" t="s">
         <v>4</v>
       </c>
@@ -1368,81 +1371,101 @@
     </row>
     <row r="22" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
+      <c r="D22" s="8">
+        <v>297</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>5</v>
+      </c>
       <c r="L22" s="8"/>
     </row>
     <row r="23" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="D23" s="8">
-        <v>210</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>48</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="8">
-        <v>67.099999999999994</v>
-      </c>
-      <c r="K23" s="8">
-        <v>32.9</v>
-      </c>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
     <row r="24" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="D24" s="8">
+        <v>210</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="J24" s="8">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="K24" s="8">
+        <v>32.9</v>
+      </c>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
+    <row r="25" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
@@ -1626,6 +1649,19 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="G2:I2"/>

</xml_diff>

<commit_message>
Add two additional HMC variations
</commit_message>
<xml_diff>
--- a/HighResIcons/Details.xlsx
+++ b/HighResIcons/Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Andrea\Code\EDDiscovery\EDDiscoveryData\HighResIcons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A31D49B-7BDA-40A1-9DE8-CBB21E6C58D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F244C1C-A9EB-453D-BB94-5365A2FE9926}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1C47AFF1-0F2E-4E80-9439-97C38743854E}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="59">
   <si>
     <t>Class</t>
   </si>
@@ -201,6 +201,12 @@
   </si>
   <si>
     <t>NWWv4</t>
+  </si>
+  <si>
+    <t>HMCv13</t>
+  </si>
+  <si>
+    <t>hmcV14</t>
   </si>
 </sst>
 </file>
@@ -712,10 +718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{378DFCFD-A23B-459A-BDF7-1A47346AC4C8}">
-  <dimension ref="B1:L40"/>
+  <dimension ref="B1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +729,7 @@
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="32.140625" customWidth="1"/>
     <col min="7" max="7" width="18.42578125" customWidth="1"/>
     <col min="8" max="8" width="19.42578125" customWidth="1"/>
@@ -1173,226 +1179,222 @@
     </row>
     <row r="16" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D16" s="8">
-        <v>259</v>
+        <v>677</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>3</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8">
+        <v>67.2</v>
+      </c>
+      <c r="K16" s="8">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="L16" s="8"/>
     </row>
     <row r="17" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D17" s="8">
-        <v>257</v>
+        <v>1230</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>5</v>
+      <c r="J17" s="8">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="K17" s="8">
+        <v>34.1</v>
       </c>
       <c r="L17" s="8"/>
     </row>
     <row r="18" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D18" s="8">
-        <v>225</v>
+        <v>259</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>17</v>
       </c>
       <c r="H18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8">
-        <v>67.7</v>
-      </c>
-      <c r="K18" s="8">
-        <v>32.9</v>
-      </c>
-      <c r="L18" s="8"/>
+      <c r="J18" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="L18" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D19" s="8">
-        <v>387</v>
+        <v>257</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="J19" s="8">
-        <v>67.3</v>
-      </c>
-      <c r="K19" s="8">
-        <v>32.700000000000003</v>
+        <v>48</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="L19" s="8"/>
     </row>
     <row r="20" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="8">
-        <v>304</v>
+        <v>225</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H20" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="I20" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="J20" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="L20" s="8" t="s">
-        <v>3</v>
-      </c>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8">
+        <v>67.7</v>
+      </c>
+      <c r="K20" s="8">
+        <v>32.9</v>
+      </c>
+      <c r="L20" s="8"/>
     </row>
     <row r="21" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>40</v>
       </c>
       <c r="D21" s="8">
-        <v>299</v>
+        <v>387</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="H21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>5</v>
+      <c r="I21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="8">
+        <v>67.3</v>
+      </c>
+      <c r="K21" s="8">
+        <v>32.700000000000003</v>
       </c>
       <c r="L21" s="8"/>
     </row>
     <row r="22" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D22" s="8">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="J22" s="8" t="s">
         <v>4</v>
@@ -1400,62 +1402,80 @@
       <c r="K22" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L22" s="8"/>
+      <c r="L22" s="8" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="23" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
+        <v>40</v>
+      </c>
+      <c r="D23" s="8">
+        <v>299</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
+      <c r="J23" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>5</v>
+      </c>
       <c r="L23" s="8"/>
     </row>
     <row r="24" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D24" s="8">
-        <v>210</v>
+        <v>297</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>14</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8">
-        <v>67.099999999999994</v>
-      </c>
-      <c r="K24" s="8">
-        <v>32.9</v>
+        <v>25</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="L24" s="8"/>
     </row>
     <row r="25" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
@@ -1467,31 +1487,53 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-    </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
+    <row r="26" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="8">
+        <v>210</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="K26" s="8">
+        <v>32.9</v>
+      </c>
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+      <c r="L27" s="8"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -1662,6 +1704,32 @@
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
     </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="G2:I2"/>

</xml_diff>